<commit_message>
Add ticket autofill script for Framework_Path and Roadmap_Milestone
</commit_message>
<xml_diff>
--- a/data/Project_Aion_PM_System.xlsx
+++ b/data/Project_Aion_PM_System.xlsx
@@ -1096,7 +1096,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="A4" s="15" t="inlineStr">
         <is>
@@ -2685,7 +2684,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:CB19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -3248,6 +3247,14 @@
       <c r="N10" s="5" t="n"/>
       <c r="O10" s="5" t="n"/>
       <c r="P10" s="5" t="n"/>
+      <c r="R10">
+        <f>IF(Q10="","",IFERROR(XLOOKUP(Q10,'99_Validation'!$A$2:$A$16,'99_Validation'!$C$2:$C$16,""),""))</f>
+        <v/>
+      </c>
+      <c r="S10">
+        <f>IF(J10="","", "Q"&amp;ROUNDUP(MONTH(J10)/3,0)&amp;"_"&amp;TEXT(J10,"yyyy"))</f>
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="n"/>
@@ -3266,6 +3273,14 @@
       <c r="N11" s="5" t="n"/>
       <c r="O11" s="5" t="n"/>
       <c r="P11" s="5" t="n"/>
+      <c r="R11">
+        <f>IF(Q11="","",IFERROR(XLOOKUP(Q11,'99_Validation'!$A$2:$A$16,'99_Validation'!$C$2:$C$16,""),""))</f>
+        <v/>
+      </c>
+      <c r="S11">
+        <f>IF(J11="","", "Q"&amp;ROUNDUP(MONTH(J11)/3,0)&amp;"_"&amp;TEXT(J11,"yyyy"))</f>
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="n"/>
@@ -3284,6 +3299,14 @@
       <c r="N12" s="5" t="n"/>
       <c r="O12" s="5" t="n"/>
       <c r="P12" s="5" t="n"/>
+      <c r="R12">
+        <f>IF(Q12="","",IFERROR(XLOOKUP(Q12,'99_Validation'!$A$2:$A$16,'99_Validation'!$C$2:$C$16,""),""))</f>
+        <v/>
+      </c>
+      <c r="S12">
+        <f>IF(J12="","", "Q"&amp;ROUNDUP(MONTH(J12)/3,0)&amp;"_"&amp;TEXT(J12,"yyyy"))</f>
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="n"/>
@@ -3302,6 +3325,14 @@
       <c r="N13" s="5" t="n"/>
       <c r="O13" s="5" t="n"/>
       <c r="P13" s="5" t="n"/>
+      <c r="R13">
+        <f>IF(Q13="","",IFERROR(XLOOKUP(Q13,'99_Validation'!$A$2:$A$16,'99_Validation'!$C$2:$C$16,""),""))</f>
+        <v/>
+      </c>
+      <c r="S13">
+        <f>IF(J13="","", "Q"&amp;ROUNDUP(MONTH(J13)/3,0)&amp;"_"&amp;TEXT(J13,"yyyy"))</f>
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="n"/>
@@ -3320,6 +3351,14 @@
       <c r="N14" s="5" t="n"/>
       <c r="O14" s="5" t="n"/>
       <c r="P14" s="5" t="n"/>
+      <c r="R14">
+        <f>IF(Q14="","",IFERROR(XLOOKUP(Q14,'99_Validation'!$A$2:$A$16,'99_Validation'!$C$2:$C$16,""),""))</f>
+        <v/>
+      </c>
+      <c r="S14">
+        <f>IF(J14="","", "Q"&amp;ROUNDUP(MONTH(J14)/3,0)&amp;"_"&amp;TEXT(J14,"yyyy"))</f>
+        <v/>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="n"/>
@@ -3338,6 +3377,14 @@
       <c r="N15" s="5" t="n"/>
       <c r="O15" s="5" t="n"/>
       <c r="P15" s="5" t="n"/>
+      <c r="R15">
+        <f>IF(Q15="","",IFERROR(XLOOKUP(Q15,'99_Validation'!$A$2:$A$16,'99_Validation'!$C$2:$C$16,""),""))</f>
+        <v/>
+      </c>
+      <c r="S15">
+        <f>IF(J15="","", "Q"&amp;ROUNDUP(MONTH(J15)/3,0)&amp;"_"&amp;TEXT(J15,"yyyy"))</f>
+        <v/>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="n"/>
@@ -3356,6 +3403,14 @@
       <c r="N16" s="5" t="n"/>
       <c r="O16" s="5" t="n"/>
       <c r="P16" s="5" t="n"/>
+      <c r="R16">
+        <f>IF(Q16="","",IFERROR(XLOOKUP(Q16,'99_Validation'!$A$2:$A$16,'99_Validation'!$C$2:$C$16,""),""))</f>
+        <v/>
+      </c>
+      <c r="S16">
+        <f>IF(J16="","", "Q"&amp;ROUNDUP(MONTH(J16)/3,0)&amp;"_"&amp;TEXT(J16,"yyyy"))</f>
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="n"/>
@@ -3374,6 +3429,14 @@
       <c r="N17" s="5" t="n"/>
       <c r="O17" s="5" t="n"/>
       <c r="P17" s="5" t="n"/>
+      <c r="R17">
+        <f>IF(Q17="","",IFERROR(XLOOKUP(Q17,'99_Validation'!$A$2:$A$16,'99_Validation'!$C$2:$C$16,""),""))</f>
+        <v/>
+      </c>
+      <c r="S17">
+        <f>IF(J17="","", "Q"&amp;ROUNDUP(MONTH(J17)/3,0)&amp;"_"&amp;TEXT(J17,"yyyy"))</f>
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="n"/>
@@ -3392,6 +3455,14 @@
       <c r="N18" s="5" t="n"/>
       <c r="O18" s="5" t="n"/>
       <c r="P18" s="5" t="n"/>
+      <c r="R18">
+        <f>IF(Q18="","",IFERROR(XLOOKUP(Q18,'99_Validation'!$A$2:$A$16,'99_Validation'!$C$2:$C$16,""),""))</f>
+        <v/>
+      </c>
+      <c r="S18">
+        <f>IF(J18="","", "Q"&amp;ROUNDUP(MONTH(J18)/3,0)&amp;"_"&amp;TEXT(J18,"yyyy"))</f>
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="n"/>
@@ -3410,6 +3481,14 @@
       <c r="N19" s="5" t="n"/>
       <c r="O19" s="5" t="n"/>
       <c r="P19" s="5" t="n"/>
+      <c r="R19">
+        <f>IF(Q19="","",IFERROR(XLOOKUP(Q19,'99_Validation'!$A$2:$A$16,'99_Validation'!$C$2:$C$16,""),""))</f>
+        <v/>
+      </c>
+      <c r="S19">
+        <f>IF(J19="","", "Q"&amp;ROUNDUP(MONTH(J19)/3,0)&amp;"_"&amp;TEXT(J19,"yyyy"))</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4156,7 +4235,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4175,6 +4254,11 @@
           <t>Allowed_Roadmap_Milestones</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Framework_Path_By_Realm</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4187,6 +4271,11 @@
           <t>Q1_2026</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Project_Aion/00_Triage_Inbox</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4199,6 +4288,11 @@
           <t>Q2_2026</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Project_Aion/01_Project_Framework</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4211,6 +4305,11 @@
           <t>Q3_2026</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Project_Aion/02_Glass_Cockpit_GUI</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4223,6 +4322,11 @@
           <t>Q4_2026</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Project_Aion/03_Artifacts</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4230,6 +4334,11 @@
           <t>04_Admin_Automation_AWACS</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Project_Aion/04_Admin_Automation_AWACS</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -4237,6 +4346,11 @@
           <t>05_IT_Infrastructure</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Project_Aion/05_IT_Infrastructure</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -4244,6 +4358,11 @@
           <t>06_Databases</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Project_Aion/06_Databases</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -4251,6 +4370,11 @@
           <t>07_Expert_Systems</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Project_Aion/07_Expert_Systems</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4258,6 +4382,11 @@
           <t>08_Modelling_Feature_Design_and_Engineering</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Project_Aion/08_Modelling_Feature_Design_and_Engineering</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -4265,6 +4394,11 @@
           <t>09_ML_AI_Systems</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Project_Aion/09_ML_AI_Systems</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -4272,6 +4406,11 @@
           <t>10_Model_Simulation_Backtesting</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Project_Aion/10_Model_Simulation_Backtesting</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -4279,6 +4418,11 @@
           <t>11_Trading_Strategies</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Project_Aion/11_Trading_Strategies</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -4286,6 +4430,11 @@
           <t>12_Trading_Engines</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Project_Aion/12_Trading_Engines</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -4293,6 +4442,11 @@
           <t>13_Business_Intelligence</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Project_Aion/13_Business_Intelligence</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -4300,7 +4454,13 @@
           <t>Framework_Directory_Spec__legacy</t>
         </is>
       </c>
-    </row>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Project_Aion/Framework_Directory_Spec__legacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="17"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
PM system aligned to Framework Index with refresh/finalize/promote scripts
</commit_message>
<xml_diff>
--- a/data/Project_Aion_PM_System.xlsx
+++ b/data/Project_Aion_PM_System.xlsx
@@ -1105,6 +1105,11 @@
       <c r="A2" t="n">
         <v>2</v>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>32_Trading_Strategies_Early_Mid_Late_Market</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>32_Trading_Strategies_Early_Mid_Late_Market</t>
@@ -1131,6 +1136,11 @@
       <c r="A4" t="n">
         <v>4</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>24_Features_Public_Live_Market</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>24_Features_Public_Live_Market</t>
@@ -1149,6 +1159,11 @@
       <c r="A5" t="n">
         <v>5</v>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1167,6 +1182,11 @@
       <c r="A6" t="n">
         <v>6</v>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1185,6 +1205,11 @@
       <c r="A7" t="n">
         <v>7</v>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1203,6 +1228,11 @@
       <c r="A8" t="n">
         <v>8</v>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1221,6 +1251,11 @@
       <c r="A9" t="n">
         <v>9</v>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1239,6 +1274,11 @@
       <c r="A10" t="n">
         <v>10</v>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1257,6 +1297,11 @@
       <c r="A11" t="n">
         <v>11</v>
       </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1275,6 +1320,11 @@
       <c r="A12" t="n">
         <v>12</v>
       </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1293,6 +1343,11 @@
       <c r="A13" t="n">
         <v>13</v>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1311,6 +1366,11 @@
       <c r="A14" t="n">
         <v>14</v>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1329,6 +1389,11 @@
       <c r="A15" t="n">
         <v>15</v>
       </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>07_Databases</t>
@@ -1346,6 +1411,11 @@
     <row r="16">
       <c r="A16" t="n">
         <v>16</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1411,6 +1481,11 @@
       <c r="A2" t="n">
         <v>2</v>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10_Pulse_Race_Status_Bet_Triggers</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>10_Pulse_Race_Status_Bet_Triggers</t>
@@ -1437,6 +1512,11 @@
       <c r="A4" t="n">
         <v>4</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>05_Glass_Cockpit_GUI</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>05_Glass_Cockpit_GUI</t>
@@ -1455,6 +1535,11 @@
       <c r="A5" t="n">
         <v>5</v>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>14_ML_XGBOOST</t>
@@ -1473,6 +1558,11 @@
       <c r="A6" t="n">
         <v>6</v>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>14_ML_XGBOOST</t>
@@ -1491,6 +1581,11 @@
       <c r="A7" t="n">
         <v>7</v>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>14_ML_XGBOOST</t>
@@ -1509,6 +1604,11 @@
       <c r="A8" t="n">
         <v>8</v>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>14_ML_XGBOOST</t>
@@ -1526,6 +1626,11 @@
     <row r="9">
       <c r="A9" t="n">
         <v>9</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -2571,9 +2676,12 @@
       <formula>$F5="In progress"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation sqref="H5:H17" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Not started,In progress,Blocked,Ready for review,Done"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K5000 T2:T5000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=Framework_Index!$A$2:$A$44</formula1>
     </dataValidation>
     <dataValidation sqref="K2:K5000 T2:T5000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>=Framework_Index!$A$2:$A$44</formula1>
@@ -4525,7 +4633,7 @@
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
   </mergeCells>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation sqref="F5:F200" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"P0,P1,P2,P3"</formula1>
     </dataValidation>
@@ -4540,6 +4648,9 @@
     </dataValidation>
     <dataValidation sqref="S5:S19" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>'99_Validation'!$B$2:$B$5</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K5000 T2:T5000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=Framework_Index!$A$2:$A$44</formula1>
     </dataValidation>
     <dataValidation sqref="K2:K5000 T2:T5000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>=Framework_Index!$A$2:$A$44</formula1>
@@ -5941,7 +6052,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -5964,7 +6075,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -6006,7 +6117,7 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -6058,7 +6169,7 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -6172,7 +6283,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -6276,7 +6387,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>

</xml_diff>